<commit_message>
Converted to python3, Solved some bugs
</commit_message>
<xml_diff>
--- a/example/excel.xlsx
+++ b/example/excel.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\excel_validator\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john.elmasry\excel_validator\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B3DE88-0A72-4827-A9F5-E27796C20120}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6474"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -113,7 +114,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -489,23 +490,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.578125" customWidth="1"/>
-    <col min="3" max="3" width="12.734375" customWidth="1"/>
-    <col min="7" max="7" width="16.9453125" customWidth="1"/>
-    <col min="10" max="10" width="12.3125" customWidth="1"/>
-    <col min="11" max="11" width="12.62890625" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -546,7 +548,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -584,7 +586,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -619,7 +621,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -639,7 +641,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -655,7 +657,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>